<commit_message>
Minor improvement to control file and fix group for God and scripture in template
</commit_message>
<xml_diff>
--- a/Glyssen/Resources/CharacterGroups.xlsx
+++ b/Glyssen/Resources/CharacterGroups.xlsx
@@ -1638,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O52" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:AG82"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12287,7 +12287,7 @@
         <v>8946</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="E111" s="6">
         <v>1</v>

</xml_diff>